<commit_message>
visualization added to frontend
</commit_message>
<xml_diff>
--- a/Auto_Binalysis_Backend/analysis/Tested_file/MemberCardAnalysisTest_output.xlsx
+++ b/Auto_Binalysis_Backend/analysis/Tested_file/MemberCardAnalysisTest_output.xlsx
@@ -2661,7 +2661,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -17689,7 +17689,7 @@
       </c>
       <c r="H575" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>